<commit_message>
Simulation with and without solar production running properly
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/trey_power_network_simu.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/trey_power_network_simu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bus" sheetId="1" state="visible" r:id="rId1"/>
@@ -2372,7 +2372,7 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -2499,8 +2499,8 @@
   </sheetPr>
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelCol="0"/>

</xml_diff>